<commit_message>
made some changes to the exel data sheet
</commit_message>
<xml_diff>
--- a/server/details.xlsx
+++ b/server/details.xlsx
@@ -92,7 +92,7 @@
         <family val="1"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">Alpinia galanga </t>
+      <t xml:space="preserve">Alpinia Galanga </t>
     </r>
     <r>
       <rPr>
@@ -128,7 +128,7 @@
         <family val="1"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">Artocarpus heterophyllus </t>
+      <t xml:space="preserve">Artocarpus Heterophyllus </t>
     </r>
     <r>
       <rPr>
@@ -164,7 +164,7 @@
         <family val="1"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">Azadirachta indica </t>
+      <t xml:space="preserve">Azadirachta Indica </t>
     </r>
     <r>
       <rPr>
@@ -200,7 +200,7 @@
         <family val="1"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">Basella alba </t>
+      <t xml:space="preserve">Basella Alba </t>
     </r>
     <r>
       <rPr>
@@ -236,7 +236,7 @@
         <family val="1"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">Brassica juncea </t>
+      <t xml:space="preserve">Brassica Juncea </t>
     </r>
     <r>
       <rPr>
@@ -272,7 +272,7 @@
         <family val="1"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">Carissa carandas </t>
+      <t xml:space="preserve">Carissa Carandas </t>
     </r>
     <r>
       <rPr>
@@ -305,7 +305,7 @@
         <family val="1"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">Citrus limon </t>
+      <t xml:space="preserve">Citrus Limon </t>
     </r>
     <r>
       <rPr>
@@ -335,7 +335,7 @@
         <family val="1"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">Ficus religiosa </t>
+      <t xml:space="preserve">Ficus Religiosa </t>
     </r>
     <r>
       <rPr>
@@ -365,7 +365,7 @@
         <family val="1"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">Jasminum spp </t>
+      <t xml:space="preserve">Jasminum </t>
     </r>
     <r>
       <rPr>
@@ -467,7 +467,7 @@
         <family val="1"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">Mentha spp </t>
+      <t xml:space="preserve">Mentha </t>
     </r>
     <r>
       <rPr>
@@ -497,7 +497,7 @@
         <family val="1"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">Moringa oleifera </t>
+      <t xml:space="preserve">Moringa Oleifera </t>
     </r>
     <r>
       <rPr>
@@ -527,7 +527,7 @@
         <family val="1"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">Ocimum tenuiflorum </t>
+      <t xml:space="preserve">Ocimum Tenuiflorum </t>
     </r>
     <r>
       <rPr>
@@ -557,7 +557,7 @@
         <family val="1"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">Piper betle </t>
+      <t xml:space="preserve">Piper Betle </t>
     </r>
     <r>
       <rPr>
@@ -587,7 +587,7 @@
         <family val="1"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">Psidium guajava</t>
+      <t xml:space="preserve">Psidium Guajava</t>
     </r>
     <r>
       <rPr>
@@ -631,7 +631,7 @@
         <family val="1"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">Psidium guajava </t>
+      <t xml:space="preserve">Psidium Guajava </t>
     </r>
     <r>
       <rPr>
@@ -661,7 +661,7 @@
         <family val="1"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">Punica granatum </t>
+      <t xml:space="preserve">Punica Granatum </t>
     </r>
     <r>
       <rPr>
@@ -724,7 +724,7 @@
         <family val="1"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">Santalum album</t>
+      <t xml:space="preserve">Santalum Album</t>
     </r>
     <r>
       <rPr>
@@ -768,7 +768,7 @@
         <family val="1"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">Syzygium cumini </t>
+      <t xml:space="preserve">Syzygium Cumini </t>
     </r>
     <r>
       <rPr>
@@ -801,7 +801,7 @@
         <family val="1"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">Syzygium jambos </t>
+      <t xml:space="preserve">Syzygium Jambos </t>
     </r>
     <r>
       <rPr>
@@ -834,7 +834,7 @@
         <family val="1"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">Zingiber officinale roscoe </t>
+      <t xml:space="preserve">Zingiber officinale Roscoe </t>
     </r>
     <r>
       <rPr>
@@ -980,55 +980,55 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1051,8 +1051,8 @@
   </sheetPr>
   <dimension ref="A1:AE490"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="66" zoomScaleNormal="66" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B13" activeCellId="0" sqref="B13"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="66" zoomScaleNormal="66" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B24" activeCellId="0" sqref="B24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>